<commit_message>
tiny change to plots
</commit_message>
<xml_diff>
--- a/plot_tables.xlsx
+++ b/plot_tables.xlsx
@@ -51,10 +51,6 @@
     <t>Pearson</t>
   </si>
   <si>
-    <t>NP
-(Tanimoto)</t>
-  </si>
-  <si>
     <t>NC-IDF
 (Tanimoto)</t>
   </si>
@@ -69,6 +65,10 @@
   <si>
     <t>ACL
 (Log)</t>
+  </si>
+  <si>
+    <t>NC
+(Tanimoto)</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2040,7 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>NP
+                  <c:v>NC
 (Tanimoto)</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -3648,7 +3648,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3667,9 +3667,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>

</xml_diff>